<commit_message>
Fix scenario NaNs by overriding all derived rows
</commit_message>
<xml_diff>
--- a/data/format.xlsx
+++ b/data/format.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\projects\stock_val\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\projects\stock_val_streamlit\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C9ADB29-D4BD-4062-A431-37236B0E71F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E66BB48-E961-443C-8393-6A672FC223A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C9AFF03F-ECC7-463B-B03A-921C9B3964C1}"/>
   </bookViews>
@@ -104,12 +104,6 @@
     <t>E Operated Margin</t>
   </si>
   <si>
-    <t xml:space="preserve">E Revenue </t>
-  </si>
-  <si>
-    <t xml:space="preserve">E EBITDA </t>
-  </si>
-  <si>
     <t>E Dilution (5yr)</t>
   </si>
   <si>
@@ -147,6 +141,12 @@
   </si>
   <si>
     <t>Suggested Position Size</t>
+  </si>
+  <si>
+    <t>E Revenue</t>
+  </si>
+  <si>
+    <t>E EBITDA</t>
   </si>
 </sst>
 </file>
@@ -631,8 +631,8 @@
   </sheetPr>
   <dimension ref="A2:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -808,7 +808,7 @@
     </row>
     <row r="24" spans="1:3" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B24" s="5">
         <f>B7*4*((1+B22)^5)</f>
@@ -821,7 +821,7 @@
     </row>
     <row r="25" spans="1:3" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="B25" s="5">
         <f t="shared" ref="B25:C25" si="0">B24*B23</f>
@@ -834,7 +834,7 @@
     </row>
     <row r="26" spans="1:3" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B26" s="8">
         <v>0</v>
@@ -845,7 +845,7 @@
     </row>
     <row r="27" spans="1:3" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B27" s="5">
         <f>B5*(1+B26)</f>
@@ -858,7 +858,7 @@
     </row>
     <row r="29" spans="1:3" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B29" s="5">
         <v>0</v>
@@ -869,7 +869,7 @@
     </row>
     <row r="30" spans="1:3" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B30" s="8">
         <v>0.05</v>
@@ -880,7 +880,7 @@
     </row>
     <row r="31" spans="1:3" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B31" s="8">
         <v>0.2</v>
@@ -891,7 +891,7 @@
     </row>
     <row r="32" spans="1:3" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B32" s="5">
         <f t="shared" ref="B32:C32" si="1">(B25-B29*B30)*(1-B31)</f>
@@ -904,7 +904,7 @@
     </row>
     <row r="34" spans="1:3" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B34" s="5">
         <f t="shared" ref="B34:C34" si="2">B32/B27</f>
@@ -917,7 +917,7 @@
     </row>
     <row r="35" spans="1:3" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B35" s="3">
         <v>20</v>
@@ -928,7 +928,7 @@
     </row>
     <row r="36" spans="1:3" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B36" s="5">
         <f t="shared" ref="B36:C36" si="3">B34*B35</f>
@@ -941,7 +941,7 @@
     </row>
     <row r="37" spans="1:3" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B37" s="8">
         <v>0.05</v>
@@ -952,7 +952,7 @@
     </row>
     <row r="38" spans="1:3" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B38" s="13">
         <f t="shared" ref="B38:C38" si="4">B36/((B37+1)^5)</f>
@@ -965,7 +965,7 @@
     </row>
     <row r="39" spans="1:3" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A39" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B39" s="14">
         <v>1</v>
@@ -974,7 +974,7 @@
     </row>
     <row r="40" spans="1:3" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A40" s="12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B40" s="14">
         <f ca="1">((C38*B39-B4)/(C38*B39-B38))</f>

</xml_diff>

<commit_message>
update on llm prompt and format.xlsx for tr stocks
</commit_message>
<xml_diff>
--- a/data/format.xlsx
+++ b/data/format.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\projects\stock_val_streamlit\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\projects\streamlit_apps\stock_val_streamlit\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{187DBBB7-C498-413B-BDAF-12DE7463C5B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{841F1D6B-DCFF-4935-9F84-841FA159367A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C9AFF03F-ECC7-463B-B03A-921C9B3964C1}"/>
   </bookViews>
@@ -631,8 +631,8 @@
   </sheetPr>
   <dimension ref="A2:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -944,9 +944,11 @@
         <v>29</v>
       </c>
       <c r="B37" s="8">
+        <f>IF(RIGHT(B3,3)=".IS",0.3,0.05)</f>
         <v>0.05</v>
       </c>
       <c r="C37" s="8">
+        <f>IF(RIGHT(B3,3)=".IS",0.25,0.05)</f>
         <v>0.05</v>
       </c>
     </row>

</xml_diff>